<commit_message>
startet with screipt for additional limed rivers
</commit_message>
<xml_diff>
--- a/ElvO 2024_Gen vannkjemi.xlsx
+++ b/ElvO 2024_Gen vannkjemi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://niva365-my.sharepoint.com/personal/cathrine_brecke_gundersen_niva_no/Documents/1 Projects/2022_Elveovervaakningen/RiverMonitoring_24/ElvO2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{30A9BE81-BBCC-486F-B70F-7BFAD4BEAC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B60C64D2-BBC8-4CCD-AED3-72123BC79DDB}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{30A9BE81-BBCC-486F-B70F-7BFAD4BEAC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA1140AF-7F19-47D7-B735-187CCD77C724}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C471031A-CBC8-4C30-B98E-E104F9F7BA43}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AR$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AR$246</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -487,6 +487,1741 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AC$184:$AC$195</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-33EE-4BAE-8C31-C38DF301469B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="873710016"/>
+        <c:axId val="873702456"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="873710016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873702456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="873702456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873710016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$184:$AA$195</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD80-4478-92C5-8C1E53ABCB7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="873746376"/>
+        <c:axId val="873758616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="873746376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873758616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="873758616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873746376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>399317</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>106240</xdr:colOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B42C7C9-D87B-1C71-4EB1-96578C7FA2A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>135547</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>137746</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>450604</xdr:colOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>23446</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D53D3A27-0B1A-90EE-30E2-37C8C1BCF7CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -804,10 +2539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B1B0E1-4D0F-415D-B609-1A0182A6E09A}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AR246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AA184" sqref="AA184:AA195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +2688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40411</v>
       </c>
@@ -1071,7 +2807,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40411</v>
       </c>
@@ -1163,7 +2899,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40411</v>
       </c>
@@ -1255,7 +2991,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40411</v>
       </c>
@@ -1374,7 +3110,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40411</v>
       </c>
@@ -1466,7 +3202,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>40411</v>
       </c>
@@ -1558,7 +3294,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>40411</v>
       </c>
@@ -1677,7 +3413,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>40411</v>
       </c>
@@ -1769,7 +3505,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40411</v>
       </c>
@@ -1888,7 +3624,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>40411</v>
       </c>
@@ -1980,7 +3716,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>40411</v>
       </c>
@@ -2072,7 +3808,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>40352</v>
       </c>
@@ -2167,7 +3903,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>40352</v>
       </c>
@@ -2289,7 +4025,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>40352</v>
       </c>
@@ -2384,7 +4120,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>40352</v>
       </c>
@@ -2479,7 +4215,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>40352</v>
       </c>
@@ -2601,7 +4337,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>40352</v>
       </c>
@@ -2696,7 +4432,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>40352</v>
       </c>
@@ -2791,7 +4527,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>40352</v>
       </c>
@@ -2886,7 +4622,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>40352</v>
       </c>
@@ -2981,7 +4717,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>40352</v>
       </c>
@@ -3076,7 +4812,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>40352</v>
       </c>
@@ -3171,7 +4907,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>40352</v>
       </c>
@@ -3293,7 +5029,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>40352</v>
       </c>
@@ -3388,7 +5124,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>40352</v>
       </c>
@@ -3510,7 +5246,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>40352</v>
       </c>
@@ -3605,7 +5341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>40352</v>
       </c>
@@ -3700,7 +5436,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>40358</v>
       </c>
@@ -3792,7 +5528,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>40358</v>
       </c>
@@ -3884,7 +5620,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>40358</v>
       </c>
@@ -4015,7 +5751,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>40358</v>
       </c>
@@ -4107,7 +5843,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>40358</v>
       </c>
@@ -4238,7 +5974,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>40358</v>
       </c>
@@ -4330,7 +6066,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>40358</v>
       </c>
@@ -4422,7 +6158,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>40358</v>
       </c>
@@ -4553,7 +6289,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>40358</v>
       </c>
@@ -4645,7 +6381,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>40358</v>
       </c>
@@ -4776,7 +6512,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>40358</v>
       </c>
@@ -4868,7 +6604,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40358</v>
       </c>
@@ -4960,7 +6696,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40372</v>
       </c>
@@ -5055,7 +6791,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40372</v>
       </c>
@@ -5189,7 +6925,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40372</v>
       </c>
@@ -5284,7 +7020,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40372</v>
       </c>
@@ -5379,7 +7115,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>40372</v>
       </c>
@@ -5513,7 +7249,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>40372</v>
       </c>
@@ -5608,7 +7344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>40372</v>
       </c>
@@ -5703,7 +7439,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>40372</v>
       </c>
@@ -5837,7 +7573,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>40372</v>
       </c>
@@ -5932,7 +7668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>40372</v>
       </c>
@@ -6066,7 +7802,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>40372</v>
       </c>
@@ -6161,7 +7897,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>40372</v>
       </c>
@@ -6256,7 +7992,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>40373</v>
       </c>
@@ -6351,7 +8087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>40373</v>
       </c>
@@ -6485,7 +8221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>40373</v>
       </c>
@@ -6580,7 +8316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>40373</v>
       </c>
@@ -6675,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>40373</v>
       </c>
@@ -6809,7 +8545,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>40373</v>
       </c>
@@ -6904,7 +8640,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>40373</v>
       </c>
@@ -6999,7 +8735,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>40373</v>
       </c>
@@ -7133,7 +8869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>40373</v>
       </c>
@@ -7228,7 +8964,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>40373</v>
       </c>
@@ -7362,7 +9098,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>40373</v>
       </c>
@@ -7454,7 +9190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>40373</v>
       </c>
@@ -7549,7 +9285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>40374</v>
       </c>
@@ -7641,7 +9377,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>40374</v>
       </c>
@@ -7760,7 +9496,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>40374</v>
       </c>
@@ -7852,7 +9588,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>40374</v>
       </c>
@@ -7944,7 +9680,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>40374</v>
       </c>
@@ -8063,7 +9799,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>40374</v>
       </c>
@@ -8155,7 +9891,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>40374</v>
       </c>
@@ -8247,7 +9983,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>40374</v>
       </c>
@@ -8366,7 +10102,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>40374</v>
       </c>
@@ -8458,7 +10194,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>40374</v>
       </c>
@@ -8577,7 +10313,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>40374</v>
       </c>
@@ -8669,7 +10405,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>40374</v>
       </c>
@@ -8761,7 +10497,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>40375</v>
       </c>
@@ -8856,7 +10592,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>40375</v>
       </c>
@@ -8978,7 +10714,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>40375</v>
       </c>
@@ -9073,7 +10809,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>40375</v>
       </c>
@@ -9168,7 +10904,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>40375</v>
       </c>
@@ -9290,7 +11026,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>40375</v>
       </c>
@@ -9385,7 +11121,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>40375</v>
       </c>
@@ -9480,7 +11216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>40375</v>
       </c>
@@ -9602,7 +11338,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>40375</v>
       </c>
@@ -9697,7 +11433,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>40375</v>
       </c>
@@ -9819,7 +11555,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>40375</v>
       </c>
@@ -9914,7 +11650,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>40375</v>
       </c>
@@ -10009,7 +11745,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>40360</v>
       </c>
@@ -10101,7 +11837,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>40360</v>
       </c>
@@ -10232,7 +11968,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>40360</v>
       </c>
@@ -10324,7 +12060,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>40360</v>
       </c>
@@ -10416,7 +12152,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>40360</v>
       </c>
@@ -10547,7 +12283,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>40360</v>
       </c>
@@ -10639,7 +12375,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>40360</v>
       </c>
@@ -10731,7 +12467,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>40360</v>
       </c>
@@ -10862,7 +12598,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>40360</v>
       </c>
@@ -10954,7 +12690,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>40360</v>
       </c>
@@ -11085,7 +12821,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>40360</v>
       </c>
@@ -11177,7 +12913,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>40360</v>
       </c>
@@ -11269,7 +13005,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>62167</v>
       </c>
@@ -11364,7 +13100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>62167</v>
       </c>
@@ -11486,7 +13222,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>62167</v>
       </c>
@@ -11581,7 +13317,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>62167</v>
       </c>
@@ -11676,7 +13412,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>62167</v>
       </c>
@@ -11798,7 +13534,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>62167</v>
       </c>
@@ -11893,7 +13629,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>62167</v>
       </c>
@@ -11988,7 +13724,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>62167</v>
       </c>
@@ -12110,7 +13846,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>62167</v>
       </c>
@@ -12205,7 +13941,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>62167</v>
       </c>
@@ -12327,7 +14063,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>62167</v>
       </c>
@@ -12422,7 +14158,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>62167</v>
       </c>
@@ -12517,7 +14253,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="113" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>40383</v>
       </c>
@@ -12639,7 +14375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>40383</v>
       </c>
@@ -12734,7 +14470,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="115" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>40383</v>
       </c>
@@ -12829,7 +14565,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="116" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>40383</v>
       </c>
@@ -12951,7 +14687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>40383</v>
       </c>
@@ -13046,7 +14782,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>40383</v>
       </c>
@@ -13141,7 +14877,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>40383</v>
       </c>
@@ -13263,7 +14999,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="120" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>40383</v>
       </c>
@@ -13358,7 +15094,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>40383</v>
       </c>
@@ -13480,7 +15216,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="122" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>40383</v>
       </c>
@@ -13575,7 +15311,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>40383</v>
       </c>
@@ -13658,7 +15394,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="124" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>40361</v>
       </c>
@@ -13750,7 +15486,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="125" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>40361</v>
       </c>
@@ -13869,7 +15605,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>40361</v>
       </c>
@@ -13961,7 +15697,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>40361</v>
       </c>
@@ -14053,7 +15789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>40361</v>
       </c>
@@ -14172,7 +15908,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>40361</v>
       </c>
@@ -14264,7 +16000,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>40361</v>
       </c>
@@ -14356,7 +16092,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>40361</v>
       </c>
@@ -14475,7 +16211,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>40361</v>
       </c>
@@ -14567,7 +16303,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>40361</v>
       </c>
@@ -14686,7 +16422,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>40361</v>
       </c>
@@ -14778,7 +16514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>40361</v>
       </c>
@@ -14870,7 +16606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>40387</v>
       </c>
@@ -14962,7 +16698,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>40387</v>
       </c>
@@ -15081,7 +16817,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>40387</v>
       </c>
@@ -15173,7 +16909,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>40387</v>
       </c>
@@ -15265,7 +17001,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>40387</v>
       </c>
@@ -15384,7 +17120,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>40387</v>
       </c>
@@ -15476,7 +17212,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>40387</v>
       </c>
@@ -15568,7 +17304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>40387</v>
       </c>
@@ -15687,7 +17423,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>40387</v>
       </c>
@@ -15779,7 +17515,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="145" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>40387</v>
       </c>
@@ -15898,7 +17634,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="146" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>40387</v>
       </c>
@@ -15990,7 +17726,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="147" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>40387</v>
       </c>
@@ -16082,7 +17818,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="148" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>40391</v>
       </c>
@@ -16177,7 +17913,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="149" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>40391</v>
       </c>
@@ -16299,7 +18035,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="150" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>40391</v>
       </c>
@@ -16394,7 +18130,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="151" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>40391</v>
       </c>
@@ -16489,7 +18225,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="152" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>40391</v>
       </c>
@@ -16611,7 +18347,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="153" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>40391</v>
       </c>
@@ -16706,7 +18442,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="154" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>40391</v>
       </c>
@@ -16801,7 +18537,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="155" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>40391</v>
       </c>
@@ -16923,7 +18659,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="156" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>40391</v>
       </c>
@@ -17018,7 +18754,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="157" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>40391</v>
       </c>
@@ -17140,7 +18876,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="158" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>40391</v>
       </c>
@@ -17235,7 +18971,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="159" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>40391</v>
       </c>
@@ -17330,7 +19066,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="160" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>40365</v>
       </c>
@@ -17425,7 +19161,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="161" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>40365</v>
       </c>
@@ -17547,7 +19283,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="162" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>40365</v>
       </c>
@@ -17642,7 +19378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>40365</v>
       </c>
@@ -17737,7 +19473,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="164" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>40365</v>
       </c>
@@ -17859,7 +19595,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="165" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>40365</v>
       </c>
@@ -17954,7 +19690,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="166" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>40365</v>
       </c>
@@ -18049,7 +19785,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="167" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>40365</v>
       </c>
@@ -18171,7 +19907,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="168" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>40365</v>
       </c>
@@ -18266,7 +20002,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="169" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>40365</v>
       </c>
@@ -18388,7 +20124,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="170" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>40365</v>
       </c>
@@ -18480,7 +20216,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="171" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>40365</v>
       </c>
@@ -18575,7 +20311,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="172" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>40357</v>
       </c>
@@ -18667,7 +20403,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="173" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>40357</v>
       </c>
@@ -18786,7 +20522,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="174" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>40357</v>
       </c>
@@ -18878,7 +20614,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="175" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>40357</v>
       </c>
@@ -18970,7 +20706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>40357</v>
       </c>
@@ -19089,7 +20825,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="177" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>40357</v>
       </c>
@@ -19181,7 +20917,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="178" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>40357</v>
       </c>
@@ -19273,7 +21009,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="179" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>40357</v>
       </c>
@@ -19392,7 +21128,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="180" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>40357</v>
       </c>
@@ -19484,7 +21220,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="181" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>40357</v>
       </c>
@@ -19603,7 +21339,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="182" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>40357</v>
       </c>
@@ -19695,7 +21431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>40357</v>
       </c>
@@ -20999,7 +22735,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="196" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>69594</v>
       </c>
@@ -21094,7 +22830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>69594</v>
       </c>
@@ -21189,7 +22925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>69594</v>
       </c>
@@ -21323,7 +23059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>69594</v>
       </c>
@@ -21418,7 +23154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>69594</v>
       </c>
@@ -21552,7 +23288,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="201" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>69594</v>
       </c>
@@ -21647,7 +23383,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="202" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>69594</v>
       </c>
@@ -21781,7 +23517,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="203" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>69594</v>
       </c>
@@ -21876,7 +23612,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="204" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>69594</v>
       </c>
@@ -22010,7 +23746,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="205" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>69594</v>
       </c>
@@ -22105,7 +23841,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="206" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>69594</v>
       </c>
@@ -22200,7 +23936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>40354</v>
       </c>
@@ -22292,7 +24028,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="208" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>40354</v>
       </c>
@@ -22411,7 +24147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>40354</v>
       </c>
@@ -22503,7 +24239,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="210" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>40354</v>
       </c>
@@ -22595,7 +24331,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="211" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>40354</v>
       </c>
@@ -22714,7 +24450,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="212" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>40354</v>
       </c>
@@ -22806,7 +24542,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="213" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>40354</v>
       </c>
@@ -22898,7 +24634,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="214" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>40354</v>
       </c>
@@ -23017,7 +24753,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="215" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>40354</v>
       </c>
@@ -23109,7 +24845,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="216" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>40354</v>
       </c>
@@ -23228,7 +24964,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="217" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>40354</v>
       </c>
@@ -23320,7 +25056,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="218" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>40354</v>
       </c>
@@ -23412,7 +25148,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="219" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>40355</v>
       </c>
@@ -23504,7 +25240,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="220" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>40355</v>
       </c>
@@ -23617,7 +25353,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="221" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>40355</v>
       </c>
@@ -23709,7 +25445,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="222" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>40355</v>
       </c>
@@ -23801,7 +25537,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="223" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>40355</v>
       </c>
@@ -23920,7 +25656,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="224" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>40355</v>
       </c>
@@ -24012,7 +25748,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="225" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>40355</v>
       </c>
@@ -24104,7 +25840,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="226" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>40355</v>
       </c>
@@ -24223,7 +25959,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="227" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>40355</v>
       </c>
@@ -24315,7 +26051,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="228" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>40355</v>
       </c>
@@ -24434,7 +26170,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="229" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>40355</v>
       </c>
@@ -24526,7 +26262,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="230" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>40355</v>
       </c>
@@ -24618,7 +26354,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="231" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>40356</v>
       </c>
@@ -24713,7 +26449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>40356</v>
       </c>
@@ -24835,7 +26571,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="233" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>40356</v>
       </c>
@@ -24930,7 +26666,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="234" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>40356</v>
       </c>
@@ -25025,7 +26761,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="235" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>40356</v>
       </c>
@@ -25147,7 +26883,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="236" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>40356</v>
       </c>
@@ -25242,7 +26978,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="237" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>40356</v>
       </c>
@@ -25337,7 +27073,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="238" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>40356</v>
       </c>
@@ -25432,7 +27168,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="239" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>40356</v>
       </c>
@@ -25527,7 +27263,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="240" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>40356</v>
       </c>
@@ -25622,7 +27358,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="241" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>40356</v>
       </c>
@@ -25717,7 +27453,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="242" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>40356</v>
       </c>
@@ -25839,7 +27575,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="243" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>40356</v>
       </c>
@@ -25934,7 +27670,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="244" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>40356</v>
       </c>
@@ -26056,7 +27792,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="245" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>40356</v>
       </c>
@@ -26151,7 +27887,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="246" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:44" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>40356</v>
       </c>
@@ -26247,7 +27983,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AR1" xr:uid="{14B1B0E1-4D0F-415D-B609-1A0182A6E09A}"/>
+  <autoFilter ref="A1:AR246" xr:uid="{14B1B0E1-4D0F-415D-B609-1A0182A6E09A}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Skienselva"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>